<commit_message>
files renamed + 3 and 4 followup added
</commit_message>
<xml_diff>
--- a/followups.xlsx
+++ b/followups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrii-balitskyi/Projects/followup-sender/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F57BB9F-FF48-D644-9A8E-F2E74B98F8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98595E5E-A8D0-E04F-AEC6-19BAFC1E73DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{AE2010FE-C48F-AF4C-8590-1C7FAECB01FD}"/>
   </bookViews>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>example.com</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>EMAIL</t>
   </si>
@@ -47,19 +44,10 @@
     <t>WEBSITE</t>
   </si>
   <si>
-    <t>example2.com</t>
-  </si>
-  <si>
     <t>example3.com</t>
   </si>
   <si>
     <t>10balian10@gmail.com</t>
-  </si>
-  <si>
-    <t>balitskyi@ukr.net</t>
-  </si>
-  <si>
-    <t>a.balitskyi@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -426,54 +414,36 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>44763</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44763</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>44763</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
@@ -481,9 +451,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{61E35902-940E-5E4E-AA55-2688564AA786}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{120E94F0-16CE-2046-A203-E08231AF1469}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{ECF78893-9AC4-9A47-B1D2-D761C0D17EBE}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{ECF78893-9AC4-9A47-B1D2-D761C0D17EBE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
one sec delay added to prevent multiple simultaneous requests
</commit_message>
<xml_diff>
--- a/followups.xlsx
+++ b/followups.xlsx
@@ -1,32 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrii-balitskyi/Projects/followup-sender/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boombalia/followup-sender/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA5B2EB-FB47-E641-94C8-F6660901E500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3ED9704-54CA-0A4E-8CD0-C88B5B29F5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{AE2010FE-C48F-AF4C-8590-1C7FAECB01FD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{AE2010FE-C48F-AF4C-8590-1C7FAECB01FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -48,7 +40,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -63,6 +55,38 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -86,10 +110,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -405,16 +441,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18CE8054-3849-8E4E-915C-170BCAFF74A9}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.83203125" customWidth="1"/>
+    <col min="3" max="3" width="41.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
@@ -425,16 +465,360 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
+      <c r="A2" s="5"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="1"/>
+      <c r="A3" s="5"/>
       <c r="C3" s="2"/>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="C4" s="2"/>
+    </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="1"/>
+      <c r="A5" s="5"/>
       <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="5"/>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="5"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="5"/>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="5"/>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="5"/>
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="5"/>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="5"/>
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="4"/>
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="4"/>
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="4"/>
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="4"/>
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="4"/>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="4"/>
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+      <c r="C49" s="1"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="5"/>
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="C51" s="1"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+      <c r="C52" s="1"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="4"/>
+      <c r="C55" s="2"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="C56" s="3"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="C57" s="3"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="C58" s="3"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="C60" s="3"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+      <c r="C61" s="3"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+      <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+      <c r="C63" s="3"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1"/>
+      <c r="C64" s="3"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="1"/>
+      <c r="C65" s="2"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1"/>
+      <c r="C66" s="3"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="1"/>
+      <c r="C67" s="3"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1"/>
+      <c r="C68" s="2"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="1"/>
+      <c r="C69" s="3"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1"/>
+      <c r="C70" s="3"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="1"/>
+      <c r="C71" s="2"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1"/>
+      <c r="C72" s="2"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1"/>
+      <c r="C73" s="3"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="1"/>
+      <c r="C74" s="3"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="1"/>
+      <c r="C75" s="3"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="1"/>
+      <c r="C76" s="3"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="1"/>
+      <c r="C77" s="2"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+      <c r="C78" s="3"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1"/>
+      <c r="C79" s="2"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1"/>
+      <c r="C80" s="2"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="1"/>
+      <c r="C81" s="3"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="1"/>
+      <c r="C82" s="2"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="1"/>
+      <c r="C83" s="3"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="1"/>
+      <c r="C84" s="3"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="1"/>
+      <c r="C85" s="2"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="1"/>
+      <c r="C86" s="2"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="1"/>
+      <c r="C87" s="3"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="1"/>
+      <c r="C88" s="3"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="1"/>
+      <c r="C89" s="3"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="1"/>
+      <c r="C90" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added logic for sending emails in batches
</commit_message>
<xml_diff>
--- a/followups.xlsx
+++ b/followups.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boombalia/followup-sender/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrii-balitskyi/Projects/followup-sender/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3ED9704-54CA-0A4E-8CD0-C88B5B29F5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C28CB9D-3DA5-DB4B-B29A-75DB1D268B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{AE2010FE-C48F-AF4C-8590-1C7FAECB01FD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="25600" windowHeight="15500" xr2:uid="{AE2010FE-C48F-AF4C-8590-1C7FAECB01FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>EMAIL</t>
   </si>
@@ -34,13 +34,61 @@
   </si>
   <si>
     <t>WEBSITE</t>
+  </si>
+  <si>
+    <t>10balian10@gmail.com</t>
+  </si>
+  <si>
+    <t>a1.</t>
+  </si>
+  <si>
+    <t>a2.</t>
+  </si>
+  <si>
+    <t>a3.</t>
+  </si>
+  <si>
+    <t>a4.</t>
+  </si>
+  <si>
+    <t>a5.</t>
+  </si>
+  <si>
+    <t>a6.</t>
+  </si>
+  <si>
+    <t>a7.</t>
+  </si>
+  <si>
+    <t>a8.</t>
+  </si>
+  <si>
+    <t>a9.</t>
+  </si>
+  <si>
+    <t>a10.</t>
+  </si>
+  <si>
+    <t>a11.</t>
+  </si>
+  <si>
+    <t>a12.</t>
+  </si>
+  <si>
+    <t>a13.</t>
+  </si>
+  <si>
+    <t>a14.</t>
+  </si>
+  <si>
+    <t>a15.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,12 +130,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF444444"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -110,7 +152,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -125,7 +167,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -444,7 +485,7 @@
   <dimension ref="A1:C90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -465,64 +506,124 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="C3" s="2"/>
+      <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="C5" s="2"/>
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="C6" s="1"/>
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="C10" s="8"/>
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="C12" s="1"/>
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="C13" s="1"/>
+      <c r="A13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="C15" s="1"/>
+      <c r="A15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="C16" s="1"/>
+      <c r="A16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
@@ -821,6 +922,10 @@
       <c r="C90" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{8AA672A2-CBFD-5D4E-8BC3-3E7EAE0CDA7C}"/>
+    <hyperlink ref="C3:C16" r:id="rId2" display="10balian10@gmail.com" xr:uid="{3B53A9F3-AFED-A24C-B4EF-8154CE5AD68D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>